<commit_message>
Partially complete BOM for Sulu-ADS1299
</commit_message>
<xml_diff>
--- a/sulu-ads1299/sulu_ads1299_bom.xlsx
+++ b/sulu-ads1299/sulu_ads1299_bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Repositories\scum-dev-board\sulu-ads1299\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74464CC-96FF-4DE0-A2D9-B86710443995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A822113-D143-4318-91F8-72077AB4266C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-9240" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="105">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -174,6 +174,9 @@
     <t>10 µF ±20% 6.3V Ceramic Capacitor X5R 0402 (1005 Metric)</t>
   </si>
   <si>
+    <t>J4</t>
+  </si>
+  <si>
     <t>SCuM QFN</t>
   </si>
   <si>
@@ -183,24 +186,9 @@
     <t>Custom</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/sullins-connector-solutions/PRPC013DAAN-RC/2775281</t>
-  </si>
-  <si>
-    <t>PRPC013DAAN-RC</t>
-  </si>
-  <si>
     <t>Sullins Connector Solutions</t>
   </si>
   <si>
-    <t>J1, J2</t>
-  </si>
-  <si>
-    <t>CONN HEADER VERT 26POS 2.54MM</t>
-  </si>
-  <si>
-    <t>Connector Header Through Hole 26 position 0.100" (2.54mm)</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/sullins-connector-solutions/PRPC010SAAN-RC/2775244</t>
   </si>
   <si>
@@ -304,6 +292,60 @@
   </si>
   <si>
     <t>GRM21BR60J107ME15K</t>
+  </si>
+  <si>
+    <t>CONN SOCKET 20POS 0.1 GOLD PCB</t>
+  </si>
+  <si>
+    <t>20 Position Elevated Socket Connector 0.100" (2.54mm) Through Hole Gold</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samtec-inc/ESQ-110-24-G-D/7097691</t>
+  </si>
+  <si>
+    <t>Samtec Inc.</t>
+  </si>
+  <si>
+    <t>CONN SOCKET 10POS 0.1 GOLD PCB</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samtec-inc/ESQ-110-14-G-S/6678044</t>
+  </si>
+  <si>
+    <t>10 Position Elevated Socket Connector 0.100" (2.54mm) Through Hole Gold</t>
+  </si>
+  <si>
+    <t>ESQ-110-14-G-S</t>
+  </si>
+  <si>
+    <t>ESQ-110-24-G-D</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/RT0402BRE0750RL/5926183</t>
+  </si>
+  <si>
+    <t>RES SMD 50 OHM 0.1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>50 Ohms ±0.1% 0.063W, 1/16W Chip Resistor 0402 (1005 Metric) Thin Film</t>
+  </si>
+  <si>
+    <t>R7, R8, R9, R10, R11, R12, R13, R14</t>
+  </si>
+  <si>
+    <t>SW1</t>
   </si>
 </sst>
 </file>
@@ -1166,10 +1208,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1223,7 +1265,7 @@
         <v>24</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>3</v>
@@ -1249,25 +1291,25 @@
     </row>
     <row r="3" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I3" s="3">
         <v>7</v>
@@ -1278,25 +1320,25 @@
     </row>
     <row r="4" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="I4" s="3">
         <v>1</v>
@@ -1313,7 +1355,7 @@
         <v>46</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>13</v>
@@ -1325,7 +1367,7 @@
         <v>8</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I5" s="3">
         <v>10</v>
@@ -1335,25 +1377,25 @@
     </row>
     <row r="6" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="I6" s="3">
         <v>1</v>
@@ -1369,7 +1411,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E7" s="3">
         <v>733910060</v>
@@ -1434,72 +1476,69 @@
     </row>
     <row r="10" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>43</v>
+        <v>101</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>42</v>
+        <v>102</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="3">
-        <v>74438343022</v>
+        <v>103</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>41</v>
+        <v>100</v>
       </c>
       <c r="I10" s="3">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
     </row>
     <row r="11" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>25</v>
+        <v>40</v>
+      </c>
+      <c r="E11" s="3">
+        <v>74438343022</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>15</v>
+      <c r="H11" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="I11" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
     </row>
     <row r="12" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I12" s="3">
         <v>1</v>
@@ -1509,19 +1548,22 @@
     </row>
     <row r="13" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="I13" s="3">
         <v>1</v>
@@ -1531,117 +1573,200 @@
     </row>
     <row r="14" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>72</v>
+        <v>20</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>74</v>
+      <c r="H14" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="I14" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+    </row>
+    <row r="15" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E15" t="s">
-        <v>49</v>
-      </c>
-      <c r="I15">
+      <c r="E15" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I15" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="E16" t="s">
-        <v>51</v>
-      </c>
-      <c r="F16" t="s">
-        <v>8</v>
-      </c>
-      <c r="H16" s="1" t="s">
         <v>50</v>
       </c>
       <c r="I16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>60</v>
-      </c>
-      <c r="B17" t="s">
-        <v>59</v>
-      </c>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I18" s="3">
+        <v>1</v>
+      </c>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+    </row>
+    <row r="19" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I19" s="3">
+        <v>1</v>
+      </c>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>97</v>
+      </c>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>98</v>
+      </c>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>99</v>
+      </c>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E17" t="s">
-        <v>57</v>
-      </c>
-      <c r="F17" t="s">
-        <v>8</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I17">
+      <c r="I23">
         <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H10" r:id="rId1" xr:uid="{6BF5543E-9324-426E-A05E-DE3C4A577F0B}"/>
-    <hyperlink ref="H12" r:id="rId2" xr:uid="{1EC4E86E-D47C-4622-973C-64CA7F5FF4AA}"/>
-    <hyperlink ref="H11" r:id="rId3" xr:uid="{0B01DD8A-3997-4A8C-B042-D0235E7E2358}"/>
+    <hyperlink ref="H11" r:id="rId1" xr:uid="{6BF5543E-9324-426E-A05E-DE3C4A577F0B}"/>
+    <hyperlink ref="H13" r:id="rId2" xr:uid="{1EC4E86E-D47C-4622-973C-64CA7F5FF4AA}"/>
+    <hyperlink ref="H12" r:id="rId3" xr:uid="{0B01DD8A-3997-4A8C-B042-D0235E7E2358}"/>
     <hyperlink ref="H9" r:id="rId4" xr:uid="{E1F80F4E-F86A-4632-8550-92AA851DDFA0}"/>
     <hyperlink ref="H8" r:id="rId5" xr:uid="{AED77D91-9A40-43A2-A4C6-D80D81896EDA}"/>
     <hyperlink ref="H7" r:id="rId6" xr:uid="{DA046B72-EBDF-4999-8536-8FDB28899EEA}"/>
     <hyperlink ref="H2" r:id="rId7" xr:uid="{74E594FB-869E-4304-BA09-F1256497435B}"/>
-    <hyperlink ref="H17" r:id="rId8" xr:uid="{F159ED8D-2CAB-4E1D-9ED7-D5BF33254EB1}"/>
-    <hyperlink ref="H16" r:id="rId9" xr:uid="{E3E06297-BCFB-4337-A5D7-EF69871C797A}"/>
+    <hyperlink ref="H23" r:id="rId8" xr:uid="{F159ED8D-2CAB-4E1D-9ED7-D5BF33254EB1}"/>
+    <hyperlink ref="H19" r:id="rId9" xr:uid="{E3E06297-BCFB-4337-A5D7-EF69871C797A}"/>
     <hyperlink ref="H5" r:id="rId10" xr:uid="{90261672-F139-440C-8B8C-17EB9F730C48}"/>
-    <hyperlink ref="H14" r:id="rId11" xr:uid="{BD7ED755-FC34-4D81-8BC9-0E8F7C10635C}"/>
+    <hyperlink ref="H15" r:id="rId11" xr:uid="{BD7ED755-FC34-4D81-8BC9-0E8F7C10635C}"/>
     <hyperlink ref="H6" r:id="rId12" xr:uid="{371CC253-C125-45F4-B084-8B33831407CC}"/>
     <hyperlink ref="H4" r:id="rId13" xr:uid="{C04EB7A7-D999-4D0C-8F70-30E43677A7BB}"/>
     <hyperlink ref="H3" r:id="rId14" xr:uid="{216F26A6-FF51-4197-9F8D-85A6BB14472C}"/>
+    <hyperlink ref="H18" r:id="rId15" xr:uid="{7145ECDF-EB7F-4BA6-BE13-5FB45BECF207}"/>
+    <hyperlink ref="H10" r:id="rId16" xr:uid="{9D3A25CC-75B8-47AA-B851-BE72F41215FB}"/>
+    <hyperlink ref="H14" r:id="rId17" display="https://www.digikey.com/en/products/detail/texas-instruments/LM2775QDSGRQ1/9675908?utm_adgroup=Texas%20Instruments&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_EN_Focus%20Suppliers&amp;utm_term=&amp;utm_content=Texas%20Instruments&amp;gclid=Cj0KCQjwj7CZBhDHARIsAPPWv3c7aiWpXHenzAKn8sFqMkFxni_juonNmcSJ7Dx9oyr-PlFVMiiO4WoaAjmMEALw_wcB" xr:uid="{3357C052-7B51-4092-A76A-A3B0DF441934}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId15"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sulu-ads1299 3.3uF differential filter caps in bom
</commit_message>
<xml_diff>
--- a/sulu-ads1299/sulu_ads1299_bom.xlsx
+++ b/sulu-ads1299/sulu_ads1299_bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Repositories\scum-dev-board\sulu-ads1299\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6C83F0-5C96-41E3-8B57-98987842C2A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4501168E-8504-4457-BC16-B6E3BBAE2469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sulu_ads1299" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="138">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -265,9 +265,6 @@
     <t>C20</t>
   </si>
   <si>
-    <t>C13, C26, C27, C28, C29, C30, C_1.1_IN1, C_1.8_IN1, C_1.1_OUT1, C_1.8_OUT1</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/en/products/detail/murata-electronics/GRM21BR60J107ME15K/9887675</t>
   </si>
   <si>
@@ -428,13 +425,31 @@
   </si>
   <si>
     <t>CT11024.3F160</t>
+  </si>
+  <si>
+    <t>3.3 µF ±10% 6.3V Ceramic Capacitor X5R 0402 (1005 Metric)</t>
+  </si>
+  <si>
+    <t>C13, C26, C_1.1_IN1, C_1.8_IN1, C_1.1_OUT1, C_1.8_OUT1</t>
+  </si>
+  <si>
+    <t>C27, C28, C29, C30</t>
+  </si>
+  <si>
+    <t>CAP CER 3.3UF 6.3V X5R 0402</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/tdk-corporation/C1005X5R0J335K050BC/2443424</t>
+  </si>
+  <si>
+    <t>C1005X5R0J335K050BC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -569,6 +584,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -867,7 +890,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -910,11 +933,13 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -948,6 +973,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1268,17 +1294,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="63.5703125" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
@@ -1399,74 +1425,74 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>135</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>132</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
+        <v>134</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>137</v>
       </c>
       <c r="F5" t="s">
         <v>8</v>
       </c>
-      <c r="H5" t="s">
-        <v>58</v>
+      <c r="H5" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="I5">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>133</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="F6" t="s">
         <v>8</v>
       </c>
       <c r="H6" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7">
-        <v>733910060</v>
+        <v>77</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>81</v>
       </c>
       <c r="F7" t="s">
         <v>8</v>
       </c>
       <c r="H7" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -1474,71 +1500,71 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>106</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>105</v>
-      </c>
-      <c r="D8" t="s">
-        <v>107</v>
-      </c>
-      <c r="E8" t="s">
-        <v>109</v>
+        <v>59</v>
+      </c>
+      <c r="E8">
+        <v>733910060</v>
       </c>
       <c r="F8" t="s">
         <v>8</v>
       </c>
       <c r="H8" t="s">
-        <v>110</v>
+        <v>19</v>
       </c>
       <c r="I8">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>107</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>105</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>104</v>
+      </c>
+      <c r="D9" t="s">
+        <v>106</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
+        <v>108</v>
       </c>
       <c r="F9" t="s">
         <v>8</v>
       </c>
       <c r="H9" t="s">
-        <v>31</v>
+        <v>109</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>98</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F10" t="s">
         <v>8</v>
       </c>
       <c r="H10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -1546,82 +1572,82 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>96</v>
+        <v>97</v>
+      </c>
+      <c r="E11" t="s">
+        <v>36</v>
       </c>
       <c r="F11" t="s">
         <v>8</v>
       </c>
       <c r="H11" t="s">
-        <v>104</v>
+        <v>32</v>
       </c>
       <c r="I11">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>94</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12">
-        <v>74438343022</v>
+        <v>95</v>
       </c>
       <c r="F12" t="s">
         <v>8</v>
       </c>
       <c r="H12" t="s">
-        <v>38</v>
+        <v>103</v>
       </c>
       <c r="I12">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" t="s">
-        <v>23</v>
+        <v>37</v>
+      </c>
+      <c r="E13">
+        <v>74438343022</v>
       </c>
       <c r="F13" t="s">
         <v>8</v>
       </c>
       <c r="H13" t="s">
-        <v>103</v>
+        <v>38</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="E14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F14" t="s">
         <v>8</v>
@@ -1635,19 +1661,22 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>25</v>
       </c>
       <c r="F15" t="s">
         <v>8</v>
       </c>
       <c r="H15" t="s">
-        <v>56</v>
+        <v>101</v>
       </c>
       <c r="I15">
         <v>1</v>
@@ -1655,28 +1684,19 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="F16" t="s">
         <v>8</v>
       </c>
-      <c r="G16" t="s">
-        <v>66</v>
-      </c>
       <c r="H16" t="s">
-        <v>101</v>
+        <v>56</v>
       </c>
       <c r="I16">
         <v>1</v>
@@ -1684,13 +1704,28 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>61</v>
+      </c>
+      <c r="B17" t="s">
+        <v>62</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>63</v>
+      </c>
+      <c r="D17" t="s">
+        <v>64</v>
       </c>
       <c r="E17" t="s">
-        <v>47</v>
+        <v>65</v>
+      </c>
+      <c r="F17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" t="s">
+        <v>100</v>
       </c>
       <c r="I17">
         <v>1</v>
@@ -1698,25 +1733,13 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>111</v>
-      </c>
-      <c r="B18" t="s">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>90</v>
-      </c>
-      <c r="D18" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="E18" t="s">
-        <v>113</v>
-      </c>
-      <c r="F18" t="s">
-        <v>8</v>
-      </c>
-      <c r="H18" t="s">
-        <v>114</v>
+        <v>47</v>
       </c>
       <c r="I18">
         <v>1</v>
@@ -1724,25 +1747,25 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="D19" t="s">
-        <v>85</v>
+        <v>48</v>
       </c>
       <c r="E19" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="F19" t="s">
         <v>8</v>
       </c>
       <c r="H19" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="I19">
         <v>1</v>
@@ -1750,25 +1773,25 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" t="s">
         <v>84</v>
       </c>
-      <c r="C20" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" t="s">
-        <v>85</v>
-      </c>
       <c r="E20" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F20" t="s">
         <v>8</v>
       </c>
       <c r="H20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I20">
         <v>1</v>
@@ -1776,25 +1799,25 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>116</v>
+        <v>82</v>
       </c>
       <c r="B21" t="s">
-        <v>117</v>
+        <v>83</v>
       </c>
       <c r="C21" t="s">
-        <v>91</v>
+        <v>44</v>
       </c>
       <c r="D21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E21" t="s">
-        <v>118</v>
+        <v>88</v>
       </c>
       <c r="F21" t="s">
         <v>8</v>
       </c>
       <c r="H21" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="I21">
         <v>1</v>
@@ -1802,25 +1825,25 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B22" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D22" t="s">
-        <v>122</v>
+        <v>84</v>
       </c>
       <c r="E22" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="F22" t="s">
         <v>8</v>
       </c>
       <c r="H22" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I22">
         <v>1</v>
@@ -1828,25 +1851,25 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B23" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C23" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D23" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
       <c r="E23" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="F23" t="s">
         <v>8</v>
       </c>
       <c r="H23" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="I23">
         <v>1</v>
@@ -1854,25 +1877,25 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>126</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>123</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="D24" t="s">
         <v>48</v>
       </c>
       <c r="E24" t="s">
-        <v>50</v>
+        <v>124</v>
       </c>
       <c r="F24" t="s">
         <v>8</v>
       </c>
       <c r="H24" t="s">
-        <v>49</v>
+        <v>125</v>
       </c>
       <c r="I24">
         <v>1</v>
@@ -1880,54 +1903,81 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>128</v>
+        <v>53</v>
       </c>
       <c r="B25" t="s">
-        <v>129</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>97</v>
+        <v>51</v>
       </c>
       <c r="D25" t="s">
-        <v>131</v>
+        <v>48</v>
       </c>
       <c r="E25" t="s">
-        <v>132</v>
+        <v>50</v>
       </c>
       <c r="F25" t="s">
         <v>8</v>
       </c>
       <c r="H25" t="s">
-        <v>130</v>
+        <v>49</v>
       </c>
       <c r="I25">
         <v>1</v>
       </c>
     </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>127</v>
+      </c>
+      <c r="B26" t="s">
+        <v>128</v>
+      </c>
+      <c r="C26" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" t="s">
+        <v>130</v>
+      </c>
+      <c r="E26" t="s">
+        <v>131</v>
+      </c>
+      <c r="F26" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26" t="s">
+        <v>129</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H12" r:id="rId1" xr:uid="{6BF5543E-9324-426E-A05E-DE3C4A577F0B}"/>
-    <hyperlink ref="H14" r:id="rId2" xr:uid="{1EC4E86E-D47C-4622-973C-64CA7F5FF4AA}"/>
-    <hyperlink ref="H13" r:id="rId3" xr:uid="{0B01DD8A-3997-4A8C-B042-D0235E7E2358}"/>
-    <hyperlink ref="H10" r:id="rId4" xr:uid="{E1F80F4E-F86A-4632-8550-92AA851DDFA0}"/>
-    <hyperlink ref="H9" r:id="rId5" xr:uid="{AED77D91-9A40-43A2-A4C6-D80D81896EDA}"/>
-    <hyperlink ref="H7" r:id="rId6" xr:uid="{DA046B72-EBDF-4999-8536-8FDB28899EEA}"/>
+    <hyperlink ref="H13" r:id="rId1" xr:uid="{6BF5543E-9324-426E-A05E-DE3C4A577F0B}"/>
+    <hyperlink ref="H15" r:id="rId2" xr:uid="{1EC4E86E-D47C-4622-973C-64CA7F5FF4AA}"/>
+    <hyperlink ref="H14" r:id="rId3" xr:uid="{0B01DD8A-3997-4A8C-B042-D0235E7E2358}"/>
+    <hyperlink ref="H11" r:id="rId4" xr:uid="{E1F80F4E-F86A-4632-8550-92AA851DDFA0}"/>
+    <hyperlink ref="H10" r:id="rId5" xr:uid="{AED77D91-9A40-43A2-A4C6-D80D81896EDA}"/>
+    <hyperlink ref="H8" r:id="rId6" xr:uid="{DA046B72-EBDF-4999-8536-8FDB28899EEA}"/>
     <hyperlink ref="H2" r:id="rId7" xr:uid="{74E594FB-869E-4304-BA09-F1256497435B}"/>
-    <hyperlink ref="H24" r:id="rId8" xr:uid="{F159ED8D-2CAB-4E1D-9ED7-D5BF33254EB1}"/>
-    <hyperlink ref="H20" r:id="rId9" xr:uid="{E3E06297-BCFB-4337-A5D7-EF69871C797A}"/>
-    <hyperlink ref="H5" r:id="rId10" xr:uid="{90261672-F139-440C-8B8C-17EB9F730C48}"/>
-    <hyperlink ref="H16" r:id="rId11" xr:uid="{BD7ED755-FC34-4D81-8BC9-0E8F7C10635C}"/>
-    <hyperlink ref="H6" r:id="rId12" xr:uid="{371CC253-C125-45F4-B084-8B33831407CC}"/>
+    <hyperlink ref="H25" r:id="rId8" xr:uid="{F159ED8D-2CAB-4E1D-9ED7-D5BF33254EB1}"/>
+    <hyperlink ref="H21" r:id="rId9" xr:uid="{E3E06297-BCFB-4337-A5D7-EF69871C797A}"/>
+    <hyperlink ref="H6" r:id="rId10" xr:uid="{90261672-F139-440C-8B8C-17EB9F730C48}"/>
+    <hyperlink ref="H17" r:id="rId11" xr:uid="{BD7ED755-FC34-4D81-8BC9-0E8F7C10635C}"/>
+    <hyperlink ref="H7" r:id="rId12" xr:uid="{371CC253-C125-45F4-B084-8B33831407CC}"/>
     <hyperlink ref="H4" r:id="rId13" xr:uid="{C04EB7A7-D999-4D0C-8F70-30E43677A7BB}"/>
     <hyperlink ref="H3" r:id="rId14" xr:uid="{216F26A6-FF51-4197-9F8D-85A6BB14472C}"/>
-    <hyperlink ref="H19" r:id="rId15" xr:uid="{7145ECDF-EB7F-4BA6-BE13-5FB45BECF207}"/>
-    <hyperlink ref="H11" r:id="rId16" xr:uid="{9D3A25CC-75B8-47AA-B851-BE72F41215FB}"/>
-    <hyperlink ref="H15" r:id="rId17" display="https://www.digikey.com/en/products/detail/texas-instruments/LM2775QDSGRQ1/9675908?utm_adgroup=Texas%20Instruments&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_EN_Focus%20Suppliers&amp;utm_term=&amp;utm_content=Texas%20Instruments&amp;gclid=Cj0KCQjwj7CZBhDHARIsAPPWv3c7aiWpXHenzAKn8sFqMkFxni_juonNmcSJ7Dx9oyr-PlFVMiiO4WoaAjmMEALw_wcB" xr:uid="{3357C052-7B51-4092-A76A-A3B0DF441934}"/>
-    <hyperlink ref="H8" r:id="rId18" xr:uid="{4B7FC37A-F345-4C96-864F-340BDED2421E}"/>
-    <hyperlink ref="H21" r:id="rId19" xr:uid="{70D4DCF0-D1F8-4A62-9B9C-724138118DCF}"/>
-    <hyperlink ref="H25" r:id="rId20" xr:uid="{7E384250-9D50-4A0D-AC23-DBEBE885B911}"/>
+    <hyperlink ref="H20" r:id="rId15" xr:uid="{7145ECDF-EB7F-4BA6-BE13-5FB45BECF207}"/>
+    <hyperlink ref="H12" r:id="rId16" xr:uid="{9D3A25CC-75B8-47AA-B851-BE72F41215FB}"/>
+    <hyperlink ref="H16" r:id="rId17" display="https://www.digikey.com/en/products/detail/texas-instruments/LM2775QDSGRQ1/9675908?utm_adgroup=Texas%20Instruments&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_EN_Focus%20Suppliers&amp;utm_term=&amp;utm_content=Texas%20Instruments&amp;gclid=Cj0KCQjwj7CZBhDHARIsAPPWv3c7aiWpXHenzAKn8sFqMkFxni_juonNmcSJ7Dx9oyr-PlFVMiiO4WoaAjmMEALw_wcB" xr:uid="{3357C052-7B51-4092-A76A-A3B0DF441934}"/>
+    <hyperlink ref="H9" r:id="rId18" xr:uid="{4B7FC37A-F345-4C96-864F-340BDED2421E}"/>
+    <hyperlink ref="H22" r:id="rId19" xr:uid="{70D4DCF0-D1F8-4A62-9B9C-724138118DCF}"/>
+    <hyperlink ref="H26" r:id="rId20" xr:uid="{7E384250-9D50-4A0D-AC23-DBEBE885B911}"/>
+    <hyperlink ref="H5" r:id="rId21" xr:uid="{29CF3033-1CEE-41DB-8629-4BB92A23F340}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed ADC's input RC value and updated resitors BOM.
</commit_message>
<xml_diff>
--- a/sulu-ads1299/sulu_ads1299_bom.xlsx
+++ b/sulu-ads1299/sulu_ads1299_bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Repositories\scum-dev-board\sulu-ads1299\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liyunjie/Documents/留學/UCB_2022Fall/scum-dev-board/sulu-ads1299/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4501168E-8504-4457-BC16-B6E3BBAE2469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA8E671-87B5-9B45-9250-73DC0E70BFFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sulu_ads1299" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="139">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -310,12 +310,6 @@
     <t>J7</t>
   </si>
   <si>
-    <t>RES SMD 50 OHM 0.1% 1/16W 0402</t>
-  </si>
-  <si>
-    <t>50 Ohms ±0.1% 0.063W, 1/16W Chip Resistor 0402 (1005 Metric) Thin Film</t>
-  </si>
-  <si>
     <t>R7, R8, R9, R10, R11, R12, R13, R14</t>
   </si>
   <si>
@@ -340,9 +334,6 @@
     <t xml:space="preserve">https://www.digikey.com/en/products/detail/ablic-u-s-a-inc/S-85S1AB18-I6T1U/9489538 </t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.digikey.com/en/products/detail/yageo/RT0402BRE0750RL/5926183 </t>
-  </si>
-  <si>
     <t>R1, R2</t>
   </si>
   <si>
@@ -443,31 +434,47 @@
   </si>
   <si>
     <t>C1005X5R0J335K050BC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/yageo/RT0402DRE07200RL/1071388</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>RT0402DRE07200RL</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>RES SMD 200 OHM 0.5% 1/16W 0402</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>200 Ohms ±0.5% 0.063W, 1/16W Chip Resistor 0402 (1005 Metric) Thin Film</t>
+    <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri Light"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -475,7 +482,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -483,7 +490,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -491,35 +498,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -527,7 +534,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -535,14 +542,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -550,14 +557,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -565,7 +572,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -573,14 +580,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -588,8 +595,15 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -935,54 +949,57 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="20% - 輔色1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - 輔色2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - 輔色3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - 輔色4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - 輔色5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - 輔色6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - 輔色1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - 輔色2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - 輔色3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - 輔色4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - 輔色5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - 輔色6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - 輔色1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - 輔色2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - 輔色3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - 輔色4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - 輔色5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - 輔色6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="中等" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="合計" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="計算方式" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="連結的儲存格" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="備註" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="超連結" xfId="42" builtinId="8"/>
+    <cellStyle name="說明文字" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="輔色1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="輔色2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="輔色3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="輔色4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="輔色5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="輔色6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="標題" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="標題 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="標題 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="標題 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="標題 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="輸入" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="輸出" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="檢查儲存格" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="壞" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="警告文字" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -998,7 +1015,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1297,23 +1314,23 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.5703125" customWidth="1"/>
-    <col min="3" max="3" width="69.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.59765625" customWidth="1"/>
+    <col min="3" max="3" width="69.19921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" customWidth="1"/>
-    <col min="11" max="11" width="8.5703125" customWidth="1"/>
-    <col min="14" max="14" width="27.140625" customWidth="1"/>
+    <col min="5" max="5" width="25.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.3984375" customWidth="1"/>
+    <col min="11" max="11" width="8.59765625" customWidth="1"/>
+    <col min="14" max="14" width="27.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1342,7 +1359,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1371,7 +1388,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>72</v>
       </c>
@@ -1397,7 +1414,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -1423,30 +1440,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C5" t="s">
+        <v>131</v>
+      </c>
+      <c r="E5" t="s">
         <v>134</v>
       </c>
-      <c r="E5" t="s">
-        <v>137</v>
-      </c>
       <c r="F5" t="s">
         <v>8</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -1454,7 +1471,7 @@
         <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
@@ -1472,7 +1489,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>80</v>
       </c>
@@ -1498,7 +1515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1521,33 +1538,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E9" t="s">
         <v>105</v>
       </c>
-      <c r="C9" t="s">
-        <v>104</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
         <v>106</v>
-      </c>
-      <c r="E9" t="s">
-        <v>108</v>
-      </c>
-      <c r="F9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" t="s">
-        <v>109</v>
       </c>
       <c r="I9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1570,7 +1587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1578,7 +1595,7 @@
         <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E11" t="s">
         <v>36</v>
@@ -1593,27 +1610,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15">
       <c r="A12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" t="s">
+        <v>138</v>
+      </c>
+      <c r="C12" t="s">
         <v>93</v>
       </c>
-      <c r="B12" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" t="s">
-        <v>95</v>
+      <c r="E12" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="F12" t="s">
         <v>8</v>
       </c>
-      <c r="H12" t="s">
-        <v>103</v>
+      <c r="H12" s="1" t="s">
+        <v>135</v>
       </c>
       <c r="I12">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1636,7 +1656,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1653,13 +1673,13 @@
         <v>8</v>
       </c>
       <c r="H14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1676,13 +1696,13 @@
         <v>8</v>
       </c>
       <c r="H15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -1702,7 +1722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>61</v>
       </c>
@@ -1725,13 +1745,13 @@
         <v>66</v>
       </c>
       <c r="H17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1745,12 +1765,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B19" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C19" t="s">
         <v>89</v>
@@ -1759,19 +1779,19 @@
         <v>48</v>
       </c>
       <c r="E19" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F19" t="s">
         <v>8</v>
       </c>
       <c r="H19" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>85</v>
       </c>
@@ -1791,13 +1811,13 @@
         <v>8</v>
       </c>
       <c r="H20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>82</v>
       </c>
@@ -1817,18 +1837,18 @@
         <v>8</v>
       </c>
       <c r="H21" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B22" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C22" t="s">
         <v>90</v>
@@ -1837,50 +1857,50 @@
         <v>84</v>
       </c>
       <c r="E22" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F22" t="s">
         <v>8</v>
       </c>
       <c r="H22" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B23" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C23" t="s">
         <v>91</v>
       </c>
       <c r="D23" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E23" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F23" t="s">
         <v>8</v>
       </c>
       <c r="H23" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B24" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C24" t="s">
         <v>92</v>
@@ -1889,19 +1909,19 @@
         <v>48</v>
       </c>
       <c r="E24" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F24" t="s">
         <v>8</v>
       </c>
       <c r="H24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="I24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -1927,33 +1947,34 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" t="s">
+        <v>125</v>
+      </c>
+      <c r="C26" t="s">
+        <v>94</v>
+      </c>
+      <c r="D26" t="s">
         <v>127</v>
       </c>
-      <c r="B26" t="s">
+      <c r="E26" t="s">
         <v>128</v>
       </c>
-      <c r="C26" t="s">
-        <v>96</v>
-      </c>
-      <c r="D26" t="s">
-        <v>130</v>
-      </c>
-      <c r="E26" t="s">
-        <v>131</v>
-      </c>
       <c r="F26" t="s">
         <v>8</v>
       </c>
       <c r="H26" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="I26">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="H13" r:id="rId1" xr:uid="{6BF5543E-9324-426E-A05E-DE3C4A577F0B}"/>
     <hyperlink ref="H15" r:id="rId2" xr:uid="{1EC4E86E-D47C-4622-973C-64CA7F5FF4AA}"/>

</xml_diff>